<commit_message>
Added 4 worksheets for Sign up Page
</commit_message>
<xml_diff>
--- a/resources/web-data.xlsx
+++ b/resources/web-data.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\git\TalentScreenAutomation\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8028"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="invalidEmail" sheetId="1" r:id="rId1"/>
+    <sheet name="invalidPassword1" sheetId="2" r:id="rId2"/>
+    <sheet name="invalidPassword2" sheetId="3" r:id="rId3"/>
+    <sheet name="invalidPassword3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -19,24 +27,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>USERNAME</t>
   </si>
   <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>test3@gmail.c</t>
+  </si>
+  <si>
+    <t>test1@</t>
+  </si>
+  <si>
+    <t>test2@.com</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>abc1234</t>
+  </si>
+  <si>
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>test3@gmail.com</t>
+    <t>Abc45678901234567890</t>
+  </si>
+  <si>
+    <t>Abcdefgh</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>1234567A</t>
+  </si>
+  <si>
+    <t>ABC1234$</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Abc12345</t>
+  </si>
+  <si>
+    <t>ERROR MESSAGE</t>
+  </si>
+  <si>
+    <t>Password Required.</t>
+  </si>
+  <si>
+    <t>Must be 8-20 characters.</t>
+  </si>
+  <si>
+    <t>Must contain one upper &amp; lower case letter and a non-letter (number or symbol.)</t>
+  </si>
+  <si>
+    <t>Invalid Email Address</t>
   </si>
 </sst>
 </file>
@@ -357,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -365,57 +415,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="test1@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A3:A5" r:id="rId4" display="test1@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>12345678</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A4" r:id="rId2" display="test1@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tests for Confirmation Password
</commit_message>
<xml_diff>
--- a/resources/web-data.xlsx
+++ b/resources/web-data.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8028" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8028" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="invalidEmail" sheetId="1" r:id="rId1"/>
     <sheet name="invalidPassword1" sheetId="2" r:id="rId2"/>
     <sheet name="invalidPassword2" sheetId="3" r:id="rId3"/>
     <sheet name="invalidPassword3" sheetId="4" r:id="rId4"/>
+    <sheet name="invalidPassword4" sheetId="5" r:id="rId5"/>
+    <sheet name="invalidPassword5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>USERNAME</t>
   </si>
@@ -47,9 +49,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>abc1234</t>
-  </si>
-  <si>
     <t>PASSWORD</t>
   </si>
   <si>
@@ -87,6 +86,30 @@
   </si>
   <si>
     <t>Abc45678901234567890$</t>
+  </si>
+  <si>
+    <t>Abc1234</t>
+  </si>
+  <si>
+    <t>ABC123456$</t>
+  </si>
+  <si>
+    <t>1234ab5678</t>
+  </si>
+  <si>
+    <t>Passwords don't match.</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Abc1234$</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Abc12345</t>
+  </si>
+  <si>
+    <t>Confirmation Required. Passwords don't match.</t>
   </si>
 </sst>
 </file>
@@ -131,9 +154,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -432,7 +456,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -440,7 +464,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -448,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -456,7 +480,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -464,7 +488,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -484,22 +508,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -507,23 +531,23 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -536,7 +560,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,50 +571,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>12345678</v>
+      <c r="A3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -598,6 +622,7 @@
     <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -606,45 +631,155 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="71.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="71.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>